<commit_message>
ThePath upload test again
</commit_message>
<xml_diff>
--- a/thepath/Example.xlsx
+++ b/thepath/Example.xlsx
@@ -8,27 +8,33 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Example" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t xml:space="preserve">Mobile Number</t>
   </si>
   <si>
+    <t xml:space="preserve">Message</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">+911234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a test message.</t>
   </si>
   <si>
     <t xml:space="preserve">Kara Collins</t>
@@ -48,33 +54,28 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,16 +120,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,53 +146,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>